<commit_message>
correction religion n babies
</commit_message>
<xml_diff>
--- a/Exam/ExoTD/2020-09-29/grades.xlsx
+++ b/Exam/ExoTD/2020-09-29/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colin/Travail/Enseignements/R/Exam/ExoTD/2020-09-29/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB540C0D-FDCA-D54A-AEA0-76447EF6AB55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB7B620-A25D-9842-A954-8A8003B1C510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="2680" windowWidth="28800" windowHeight="17540" xr2:uid="{B5AD9CED-9E63-D545-AB8E-7FD645B63A4E}"/>
   </bookViews>
@@ -98,10 +98,10 @@
     <t>stack plots</t>
   </si>
   <si>
-    <t># barème</t>
-  </si>
-  <si>
     <t>arif_lubna</t>
+  </si>
+  <si>
+    <t># scale</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A3" sqref="A3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +508,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <f t="shared" ref="B2:B14" si="0">SUM(C2:J2)</f>
@@ -543,7 +543,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -574,9 +574,9 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -609,7 +609,7 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -642,7 +642,7 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -675,7 +675,7 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -708,7 +708,7 @@
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -807,7 +807,7 @@
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>

</xml_diff>